<commit_message>
update to data fitting version
</commit_message>
<xml_diff>
--- a/acid_data.xlsx
+++ b/acid_data.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ewueagles-my.sharepoint.com/personal/rmcrae_ewu_edu/Documents/titrator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ewueagles-my.sharepoint.com/personal/rmcrae_ewu_edu/Documents/titrator/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_7455A15CD2D8DFAFB1D7ED68F6B8D8842E398F2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DDC64A2-A93B-4D71-B8AE-A162FFCDB710}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_7455A15CD2D8DFAFB1D7ED68F6B8D8842E398F2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B9E5389-77DD-4091-AEFC-898D0E0E9D8F}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="23895" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35700" yWindow="2985" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="acid_names">Sheet1!$A$2:$A$137</definedName>
+    <definedName name="acid_names">Sheet1!$A$2:$A$138</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>acid</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>histidine</t>
+  </si>
+  <si>
+    <t>KHP</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -654,7 +661,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -760,7 +767,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -902,7 +909,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -910,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,612 +1015,614 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1.0999999999999999E-9</v>
-      </c>
+      <c r="A3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="10">
+        <v>3.8999999999999999E-6</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="B4" s="3">
-        <v>1E-25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5.0099999999999997E-3</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2.0000000000000001E-10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3.3E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1.85E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3">
-        <v>5.8E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="3">
         <f>10^-3.9</f>
         <v>1.2589254117941672E-4</v>
       </c>
-      <c r="C9">
+      <c r="C4">
         <f>10^-9.8</f>
         <v>1.5848931924611098E-10</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="3">
+        <f>10^-1.7</f>
+        <v>1.9952623149688792E-2</v>
+      </c>
+      <c r="C5">
+        <f>10^-8.3</f>
+        <v>5.0118723362727114E-9</v>
+      </c>
+      <c r="D5">
+        <f>10^-10.8</f>
+        <v>1.5848931924611082E-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="3">
+        <f>10^-4.25</f>
+        <v>5.6234132519034887E-5</v>
+      </c>
+      <c r="C6">
+        <f>10^-9.67</f>
+        <v>2.1379620895022245E-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="3">
+        <f>10^-2.2</f>
+        <v>6.3095734448019251E-3</v>
+      </c>
+      <c r="C7">
+        <f>10^-4.25</f>
+        <v>5.6234132519034887E-5</v>
+      </c>
+      <c r="D7">
+        <f>10^-9.67</f>
+        <v>2.1379620895022245E-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="3">
+        <f>10^-2.3</f>
+        <v>5.0118723362727212E-3</v>
+      </c>
+      <c r="C8">
+        <f>10^-9.6</f>
+        <v>2.5118864315095784E-10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="3">
+        <f>10^-9.2</f>
+        <v>6.309573444801927E-10</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3">
-        <v>0.2</v>
+        <v>1.0999999999999999E-9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>6.3E-5</v>
+        <v>1E-25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
+      <c r="A12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>1.4E-3</v>
+        <v>5.0099999999999997E-3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.0000000000000001E-10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3">
-        <v>1.4E-3</v>
+        <v>3.3E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
-        <v>1.6000000000000001E-4</v>
+        <v>1.85E-4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
-        <v>1.1E-4</v>
+        <v>5.8E-4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>3.8000000000000001E-9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
-        <v>1.3999999999999999E-9</v>
+        <v>6.3E-5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
-        <v>5.4999999999999996E-10</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
-        <v>1.5099999999999999E-5</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="C20" s="3">
-        <v>3.9999999999999998E-11</v>
+        <v>1.6000000000000001E-4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
-        <v>10</v>
+        <v>1.1E-4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3">
-        <v>1.4E-3</v>
+        <v>3.8000000000000001E-9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
-        <v>1.1000000000000001E-3</v>
+        <v>1.3999999999999999E-9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3">
-        <v>1.5E-3</v>
+        <v>5.4999999999999996E-10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3">
-        <v>1E-3</v>
+        <v>1.5099999999999999E-5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3">
-        <v>1.4E-3</v>
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3.9999999999999998E-11</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3">
-        <v>8.7000000000000001E-5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
-        <v>3.0000000000000001E-5</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3">
-        <v>3.3000000000000002E-9</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3">
-        <v>9.5999999999999999E-10</v>
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B31" s="3">
-        <v>4.2E-10</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3">
-        <v>1.58E-3</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3">
-        <v>8.2999999999999998E-5</v>
+        <v>8.7000000000000001E-5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3">
-        <v>0.01</v>
+        <v>3.0000000000000001E-5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3">
-        <v>1.2999999999999999E-4</v>
+        <v>3.3000000000000002E-9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B36" s="3">
-        <v>3.6000000000000001E-5</v>
+        <v>9.5999999999999999E-10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B37" s="3">
-        <v>7.3999999999999999E-4</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1.7E-5</v>
-      </c>
-      <c r="D37" s="3">
-        <v>3.8999999999999999E-6</v>
+        <v>4.2E-10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B38" s="3">
-        <v>7.2000000000000005E-4</v>
+        <v>1.58E-3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B39" s="3">
-        <v>2.3000000000000001E-4</v>
+        <v>8.2999999999999998E-5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1.2999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="3">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="3">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1.7E-5</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3.8999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7.2000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="3">
+        <v>2.3000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B46" s="3">
         <v>2.7999999999999998E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B47" s="3">
         <v>1.0999999999999999E-8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="3">
-        <f>10^-1.7</f>
-        <v>1.9952623149688792E-2</v>
-      </c>
-      <c r="C42">
-        <f>10^-8.3</f>
-        <v>5.0118723362727114E-9</v>
-      </c>
-      <c r="D42">
-        <f>10^-10.8</f>
-        <v>1.5848931924611082E-11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="3">
-        <v>3.8000000000000003E-8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="3">
-        <v>5.0999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="3">
-        <v>3.4999999999999998E-10</v>
-      </c>
-      <c r="C45" s="3">
-        <v>2.0000000000000001E-13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="3">
-        <v>9.3000000000000007E-6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="3">
-        <v>8.1000000000000004E-5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="3">
+        <v>3.8000000000000003E-8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="3">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="3">
+        <v>3.4999999999999998E-10</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2.0000000000000001E-13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="3">
+        <v>9.3000000000000007E-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="3">
+        <v>8.1000000000000004E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B53" s="3">
         <v>9.9999999999999998E-17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B54" s="3">
         <v>9.9999999999999995E-45</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B55" s="3">
         <v>1.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B56" s="3">
         <v>5.3999999999999998E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B57" s="3">
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B58" s="3">
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B59" s="3">
         <v>5.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B60" s="3">
         <v>1.3999999999999999E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B61" s="3">
         <v>7.2000000000000002E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B62" s="3">
         <v>1.5E-9</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B63" s="3">
         <v>5.1999999999999996E-10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B64" s="3">
         <v>1.5E-10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="3">
-        <v>1.8000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B61" s="3">
-        <f>10^-4.25</f>
-        <v>5.6234132519034887E-5</v>
-      </c>
-      <c r="C61">
-        <f>10^-9.67</f>
-        <v>2.1379620895022245E-10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B62" s="3">
-        <f>10^-2.2</f>
-        <v>6.3095734448019251E-3</v>
-      </c>
-      <c r="C62">
-        <f>10^-4.25</f>
-        <v>5.6234132519034887E-5</v>
-      </c>
-      <c r="D62">
-        <f>10^-9.67</f>
-        <v>2.1379620895022245E-10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B63" s="3">
-        <f>10^-2.3</f>
-        <v>5.0118723362727212E-3</v>
-      </c>
-      <c r="C63">
-        <f>10^-9.6</f>
-        <v>2.5118864315095784E-10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B64" s="3">
-        <f>10^-9.2</f>
-        <v>6.309573444801927E-10</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1.8000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B66" s="3">
         <v>1000000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B66" s="3">
-        <v>10000000</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" s="3">
-        <v>6.6E-4</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="3">
+        <v>6.6E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B69" s="3">
         <v>10000000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="3">
-        <v>1E-4</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70" s="3">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="C70" s="3">
-        <v>1.1999999999999999E-13</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1.1999999999999999E-13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B71" s="3">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="B72" s="3">
         <v>1E-3</v>
@@ -1621,114 +1630,114 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73" s="3">
-        <v>8.2999999999999998E-5</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74" s="3">
-        <v>2.6999999999999999E-5</v>
+        <v>8.2999999999999998E-5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" s="3">
-        <v>7.6000000000000004E-4</v>
+        <v>2.6999999999999999E-5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" s="3">
-        <v>1.4E-3</v>
+        <v>7.6000000000000004E-4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B77" s="3">
-        <v>1.3999999999999999E-4</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B78" s="3">
-        <v>1E-4</v>
+        <v>1.3999999999999999E-4</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79" s="3">
-        <v>3.4999999999999999E-9</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B80" s="3">
-        <v>1.3000000000000001E-9</v>
+        <v>3.4999999999999999E-9</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B81" s="3">
-        <v>6.3E-10</v>
+        <v>1.3000000000000001E-9</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="3">
-        <v>1.5E-3</v>
-      </c>
-      <c r="C82" s="3">
-        <v>1.9999999999999999E-6</v>
+        <v>6.3E-10</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" s="3">
-        <v>9.9999999999999994E-50</v>
+        <v>1.5E-3</v>
+      </c>
+      <c r="C83" s="3">
+        <v>1.9999999999999999E-6</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84" s="3">
-        <v>2.8999999999999998E-16</v>
+        <v>9.9999999999999994E-50</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="3">
+        <v>2.8999999999999998E-16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B85" s="3">
-        <v>8.1000000000000004E-5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="B86" s="3">
         <v>8.1000000000000004E-5</v>
@@ -1736,442 +1745,450 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="3">
+        <v>8.1000000000000004E-5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B88" s="3">
         <v>3.4E-5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B89" s="3">
         <v>1E-10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="3">
-        <v>2.1999999999999999E-10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" s="3">
-        <v>6.2000000000000006E-11</v>
+        <v>2.1999999999999999E-10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91" s="3">
-        <v>1.2E-4</v>
+        <v>6.2000000000000006E-11</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B92" s="3">
-        <v>5.3999999999999998E-5</v>
+        <v>1.2E-4</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93" s="3">
-        <v>4.1999999999999998E-5</v>
+        <v>5.3999999999999998E-5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94" s="3">
-        <v>5.0999999999999998E-11</v>
+        <v>4.1999999999999998E-5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" s="3">
-        <v>8.2999999999999998E-11</v>
+        <v>5.0999999999999998E-11</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="3">
-        <v>5.4999999999999997E-11</v>
+        <v>8.2999999999999998E-11</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="3">
-        <v>1.5999999999999999E-5</v>
+        <v>5.4999999999999997E-11</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="3">
-        <v>16</v>
+        <v>1.5999999999999999E-5</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99" s="3">
-        <v>3E-10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B100" s="3">
-        <v>0.27</v>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B102" s="3">
-        <v>6.8999999999999997E-5</v>
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B103" s="3">
-        <v>1.4000000000000001E-10</v>
+        <v>6.8999999999999997E-5</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B104" s="3">
-        <v>2.3000000000000001E-10</v>
+        <v>1.4000000000000001E-10</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B105" s="3">
-        <v>44</v>
+        <v>2.3000000000000001E-10</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B106" s="3">
-        <v>2.1000000000000001E-2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B107" s="3">
-        <v>6.1999999999999998E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108" s="3">
-        <v>3.2000000000000003E-4</v>
+        <v>6.1999999999999998E-3</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B109" s="3">
-        <v>3.8000000000000002E-4</v>
+        <v>3.2000000000000003E-4</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B110" s="3">
-        <v>5.9999999999999995E-8</v>
+        <v>3.8000000000000002E-4</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B111" s="3">
-        <v>4.1000000000000003E-9</v>
+        <v>5.9999999999999995E-8</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B112" s="3">
-        <v>7.1E-8</v>
+        <v>4.1000000000000003E-9</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B113" s="3">
-        <v>4.0000000000000002E-4</v>
+        <v>7.1E-8</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B114" s="3">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="C114" s="3">
-        <v>5.3999999999999998E-5</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B115" s="3">
-        <v>100000000</v>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C115" s="3">
+        <v>5.3999999999999998E-5</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B116" s="3">
-        <v>1E-10</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B117" s="3">
-        <v>4.8999999999999998E-5</v>
+        <v>1E-10</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B118" s="3">
-        <v>3.4699999999999998E-4</v>
+        <v>4.8999999999999998E-5</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B119" s="3">
-        <v>5.5000000000000002E-5</v>
+        <v>3.4699999999999998E-4</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B120" s="3">
-        <v>6.2000000000000003E-5</v>
+        <v>5.5000000000000002E-5</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B121" s="3">
-        <v>7.6E-3</v>
-      </c>
-      <c r="C121" s="3">
-        <v>6.1999999999999999E-8</v>
-      </c>
-      <c r="D121" s="3">
-        <v>2.2E-13</v>
+        <v>6.2000000000000003E-5</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B122" s="3">
+        <v>7.6E-3</v>
+      </c>
+      <c r="C122" s="3">
+        <v>6.1999999999999999E-8</v>
+      </c>
+      <c r="D122" s="3">
+        <v>2.2E-13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B122" s="10">
+      <c r="B123" s="10">
         <f>0.05</f>
         <v>0.05</v>
       </c>
-      <c r="C122" s="10">
+      <c r="C123" s="10">
         <f>0.0000002</f>
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B123" s="3">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="C123" s="3">
-        <v>3.8999999999999999E-6</v>
-      </c>
+      <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B124" s="3">
-        <v>2.4000000000000001E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C124" s="3">
-        <v>2.5000000000000001E-5</v>
+        <v>3.8999999999999999E-6</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B125" s="3">
-        <v>2.9E-4</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="C125" s="3">
-        <v>3.4999999999999997E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B126" s="3">
-        <v>0.56000000000000005</v>
+        <v>2.9E-4</v>
+      </c>
+      <c r="C126" s="3">
+        <v>3.4999999999999997E-5</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B127" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B127" s="3">
+      <c r="B128" s="3">
         <v>1.2999999999999999E-5</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B128" s="3">
+      <c r="B129" s="3">
         <v>1E-3</v>
       </c>
-      <c r="C128" s="3">
+      <c r="C129" s="3">
         <v>1.4999999999999999E-14</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B129" s="3">
-        <v>6.2000000000000003E-5</v>
-      </c>
-      <c r="C129" s="3">
-        <v>2.3E-6</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B130" s="3">
-        <v>1000</v>
+        <v>6.2000000000000003E-5</v>
       </c>
       <c r="C130" s="3">
-        <v>1.2E-2</v>
+        <v>2.3E-6</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" s="3">
-        <v>2.9999999999999999E-7</v>
+        <v>1000</v>
+      </c>
+      <c r="C131" s="3">
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" s="3">
-        <v>1.5E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B133" s="3">
-        <v>0.22</v>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B134" s="3">
-        <v>0.59</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B135" s="3">
-        <v>1.7000000000000001E-4</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B136" s="3">
-        <v>2.1900000000000001E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B137" s="3">
+        <v>2.1900000000000001E-4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B137" s="3">
+      <c r="B138" s="3">
         <v>0.56000000000000005</v>
       </c>
     </row>

</xml_diff>